<commit_message>
update data readme ...
</commit_message>
<xml_diff>
--- a/src/main/data/excel/28x28Grayscale.xlsx
+++ b/src/main/data/excel/28x28Grayscale.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4DCF8D-C54E-4414-8A3B-679D6C30D906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D564E6E-887E-4440-86AD-2A76BB9AEA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{F508E0F5-39E4-4B86-A9E4-99B40DC9E6CD}"/>
   </bookViews>
@@ -41,9 +41,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Copy an row from the minist data sets, click in cell A2 -&gt; RC -&gt; Paste Transpose. Should be able
+    <t>Copy an row from the minist data sets or your won, click in cell A2 -&gt; RC -&gt; Paste Transpose. Should be able
 to make out the image in the 28x28 Grid. Note the first cell in each row in the minst dataset is the
-the label which becomes the value in cell A2</t>
+the label which becomes the value in cell A2. Useful to check that your augmented data still look like the number intended.</t>
   </si>
 </sst>
 </file>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C771D19-521D-460E-9BC0-ADE73835A95C}">
   <dimension ref="A1:AP786"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AR4" sqref="AR4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>